<commit_message>
committed login test changes
</commit_message>
<xml_diff>
--- a/data/register.xlsx
+++ b/data/register.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EclipseWorkspace\Framework\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UpskillWorkspace\Framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="testexcel" sheetId="1" r:id="rId1"/>
+    <sheet name="custName" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -41,16 +42,22 @@
     <t>TestCaseID</t>
   </si>
   <si>
-    <t>athul</t>
-  </si>
-  <si>
-    <t>samepassword</t>
-  </si>
-  <si>
     <t>TC001</t>
   </si>
   <si>
     <t>TC002</t>
+  </si>
+  <si>
+    <t>invmsg</t>
+  </si>
+  <si>
+    <t>Bad credentials</t>
+  </si>
+  <si>
+    <t>dashboard</t>
+  </si>
+  <si>
+    <t>Hello Customer!!!</t>
   </si>
 </sst>
 </file>
@@ -391,19 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -413,10 +421,13 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -424,16 +435,44 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>